<commit_message>
Cambiando requisitos, modelo de equipos y tabla de miembros y equipos.
</commit_message>
<xml_diff>
--- a/guia/requisitos.xlsx
+++ b/guia/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -319,10 +319,10 @@
     <t xml:space="preserve">R28</t>
   </si>
   <si>
-    <t xml:space="preserve">Añadir miembros a un tablero.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En el contenido del tablero, habrá una sección que, por medio de un formulario, se buscará a otro usuario, que esté registrado en la aplicación. Se deberá indicar el nombre de usuario o su dirección de correo electrónico, el mismo que uso para registrarse. Una vez buscado, se añadirá dicho usuario al tablero, de manera que podrá śolo ver su contenido y añadir comentarios en las tarjetas.</t>
+    <t xml:space="preserve">Añadir miembros a un equipo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el contenido del equipo, habrá una sección que, por medio de un formulario, se buscará a otro usuario, que esté registrado en la aplicación. Se deberá indicar el nombre de usuario o su dirección de correo electrónico, el mismo que uso para registrarse. Una vez buscado, se añadirá dicho usuario al equipo y formará parte del equipo.</t>
   </si>
   <si>
     <t xml:space="preserve">R29</t>
@@ -960,19 +960,19 @@
   </sheetPr>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G86" activeCellId="0" sqref="G86"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="51.5663265306123"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="50.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2056,6 +2056,7 @@
         <v>94</v>
       </c>
       <c r="F43" s="8"/>
+      <c r="G43" s="0"/>
       <c r="H43" s="4" t="n">
         <v>42</v>
       </c>
@@ -2076,6 +2077,8 @@
       <c r="E44" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
       <c r="H44" s="4" t="n">
         <v>43</v>
       </c>
@@ -2096,6 +2099,8 @@
       <c r="E45" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
       <c r="H45" s="4" t="n">
         <v>44</v>
       </c>
@@ -2116,6 +2121,8 @@
       <c r="E46" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
       <c r="H46" s="4" t="n">
         <v>45</v>
       </c>
@@ -2136,6 +2143,8 @@
       <c r="E47" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F47" s="0"/>
+      <c r="G47" s="0"/>
       <c r="H47" s="4" t="n">
         <v>46</v>
       </c>
@@ -2156,6 +2165,8 @@
       <c r="E48" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F48" s="0"/>
+      <c r="G48" s="0"/>
       <c r="H48" s="4" t="n">
         <v>47</v>
       </c>
@@ -2176,6 +2187,8 @@
       <c r="E49" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F49" s="0"/>
+      <c r="G49" s="0"/>
       <c r="H49" s="4" t="n">
         <v>48</v>
       </c>
@@ -2187,12 +2200,15 @@
       <c r="B50" s="2" t="s">
         <v>162</v>
       </c>
+      <c r="C50" s="0"/>
       <c r="D50" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F50" s="0"/>
+      <c r="G50" s="0"/>
       <c r="H50" s="4" t="n">
         <v>49</v>
       </c>
@@ -2213,6 +2229,8 @@
       <c r="E51" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F51" s="0"/>
+      <c r="G51" s="0"/>
       <c r="H51" s="4" t="n">
         <v>50</v>
       </c>
@@ -2233,6 +2251,8 @@
       <c r="E52" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F52" s="0"/>
+      <c r="G52" s="0"/>
       <c r="H52" s="4" t="n">
         <v>51</v>
       </c>
@@ -2244,12 +2264,15 @@
       <c r="B53" s="2" t="s">
         <v>170</v>
       </c>
+      <c r="C53" s="0"/>
       <c r="D53" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F53" s="0"/>
+      <c r="G53" s="0"/>
       <c r="H53" s="4" t="n">
         <v>52</v>
       </c>
@@ -2261,12 +2284,15 @@
       <c r="B54" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="C54" s="0"/>
       <c r="D54" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F54" s="0"/>
+      <c r="G54" s="0"/>
       <c r="H54" s="4" t="n">
         <v>53</v>
       </c>
@@ -2278,12 +2304,15 @@
       <c r="B55" s="2" t="s">
         <v>174</v>
       </c>
+      <c r="C55" s="0"/>
       <c r="D55" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F55" s="0"/>
+      <c r="G55" s="0"/>
       <c r="H55" s="4" t="n">
         <v>54</v>
       </c>
@@ -2304,6 +2333,8 @@
       <c r="E56" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F56" s="0"/>
+      <c r="G56" s="0"/>
       <c r="H56" s="4" t="n">
         <v>55</v>
       </c>
@@ -2324,6 +2355,8 @@
       <c r="E57" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F57" s="0"/>
+      <c r="G57" s="0"/>
       <c r="H57" s="4" t="n">
         <v>56</v>
       </c>
@@ -2344,6 +2377,8 @@
       <c r="E58" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F58" s="0"/>
+      <c r="G58" s="0"/>
       <c r="H58" s="4" t="n">
         <v>57</v>
       </c>
@@ -2364,6 +2399,8 @@
       <c r="E59" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F59" s="0"/>
+      <c r="G59" s="0"/>
       <c r="H59" s="4" t="n">
         <v>58</v>
       </c>
@@ -2384,6 +2421,8 @@
       <c r="E60" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="F60" s="0"/>
+      <c r="G60" s="0"/>
       <c r="H60" s="4" t="n">
         <v>59</v>
       </c>

</xml_diff>